<commit_message>
update data generation code; intro to R content in slides
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Google Drive\marquette-workshop-2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boveee\OneDrive - Marquette University\marquette-workshop-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EA9C0BA-02A2-43F2-B497-7B5431932C55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{8EA9C0BA-02A2-43F2-B497-7B5431932C55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA7ADB46-F258-4B83-821B-53356213761C}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{4C3DB9C3-1D5F-438D-AEE3-1346D0A0AB8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4C3DB9C3-1D5F-438D-AEE3-1346D0A0AB8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,18 +33,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
   <si>
     <t>student-id</t>
   </si>
   <si>
-    <t>award</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>counsl Spring</t>
+  </si>
+  <si>
+    <t>counsl Fall</t>
+  </si>
+  <si>
+    <t>honors</t>
+  </si>
+  <si>
+    <t>advising</t>
+  </si>
+  <si>
+    <t>major</t>
   </si>
 </sst>
 </file>
@@ -80,8 +92,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,95 +411,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69070F67-5CFB-4C3E-B856-D81C62E8CCD5}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>